<commit_message>
redo contam for 11.8 kg girl
</commit_message>
<xml_diff>
--- a/data/tab_wfa_girls_p_0_5.xlsx
+++ b/data/tab_wfa_girls_p_0_5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesrobinson/Documents/git-repos/dried-fish/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robins64/Documents/git_repos/dried-fish/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6518053-518A-1B42-B32B-7662B75E249B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCD944A-37E4-534B-82F3-8307FCFABB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,11 +566,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -928,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1378,7 +1377,7 @@
       <c r="J8" s="1">
         <v>6.4</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="1">
         <v>6.7</v>
       </c>
       <c r="L8" s="1">
@@ -3117,62 +3116,62 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A38">
+    <row r="38" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>-0.3201</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>13.850300000000001</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>0.12919</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <v>9.5</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="1">
         <v>10.4</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="1">
         <v>11</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="1">
         <v>11.3</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="2">
         <v>11.8</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="1">
         <v>12.1</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="1">
         <v>12.7</v>
       </c>
-      <c r="L38">
+      <c r="L38" s="1">
         <v>13.9</v>
       </c>
-      <c r="M38">
+      <c r="M38" s="1">
         <v>15.1</v>
       </c>
-      <c r="N38">
+      <c r="N38" s="1">
         <v>15.9</v>
       </c>
-      <c r="O38">
+      <c r="O38" s="1">
         <v>16.399999999999999</v>
       </c>
-      <c r="P38">
+      <c r="P38" s="1">
         <v>17.3</v>
       </c>
-      <c r="Q38">
+      <c r="Q38" s="1">
         <v>17.8</v>
       </c>
-      <c r="R38">
+      <c r="R38" s="1">
         <v>19</v>
       </c>
-      <c r="S38">
+      <c r="S38" s="1">
         <v>21.2</v>
       </c>
     </row>

</xml_diff>